<commit_message>
still beginning (distance matrix, random path lengths)
</commit_message>
<xml_diff>
--- a/Data/11-square.xlsx
+++ b/Data/11-square.xlsx
@@ -24,12 +24,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>bottom-left</t>
   </si>
   <si>
@@ -43,6 +37,12 @@
   </si>
   <si>
     <t>top-right</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -393,15 +393,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>-5</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>-5</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="89" spans="3:4">
       <c r="C89">
-        <f t="shared" ref="C89:C123" si="1">C78+1</f>
+        <f t="shared" ref="C89:C122" si="1">C78+1</f>
         <v>2</v>
       </c>
       <c r="D89">
@@ -1378,7 +1378,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C122">
         <f t="shared" si="1"/>

</xml_diff>